<commit_message>
Solved Leetcode 547 L547_Number_of_ProvincesxConnectedComponents
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5016991-1F57-4A2E-A5A9-82BC24D19619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C44F051-2ECC-4BE2-AC14-611B904D5E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -127,32 +127,41 @@
     <t>1161. Maximum Level Sum of a Binary Tree</t>
   </si>
   <si>
-    <t xml:space="preserve">	
+    <t xml:space="preserve">Striver A TO Z </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurrsion </t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/traversal-techniques</t>
+  </si>
+  <si>
+    <t>Use adjacency list , visited array and  traverse queue</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/connected-components , https://leetcode.com/problems/number-of-provinces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for each unvisited node traverse all its neighbors using recurrsion and mark it as visited and return for how many unvisited you travelled </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leetcode , Striver A TO Z </t>
+  </si>
+  <si>
+    <t>Easy - Medium</t>
+  </si>
+  <si>
+    <t>547. Number of Province , 	
 Connected Components</t>
   </si>
   <si>
-    <t>https://takeuforward.org/plus/dsa/problems/connected-components</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maintain visited array and use recurrsion </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Striver A TO Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recurrsion </t>
-  </si>
-  <si>
-    <t>BFS</t>
-  </si>
-  <si>
-    <t>https://takeuforward.org/plus/dsa/problems/traversal-techniques</t>
-  </si>
-  <si>
-    <t>Use adjacency list , visited array and  traverse queue</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -830,7 +839,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -879,49 +888,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>37</v>
+      <c r="G2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CBDDA4D9-3DA6-42F4-BD81-6766CE6059E4}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://takeuforward.org/plus/dsa/problems/connected-components" xr:uid="{CBDDA4D9-3DA6-42F4-BD81-6766CE6059E4}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{D4ED72D4-0FD6-484E-AD61-CDBC7D2FE01F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented BFS on adjacency matrix
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C44F051-2ECC-4BE2-AC14-611B904D5E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9B779E-0F96-4286-8AFC-CC8F6CA63359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Recurrsion, DFS, Tree</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -905,7 +908,7 @@
         <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
solved L542_01_Matrix and added TC & SC for all problems in the sheet
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA332B70-7F2B-49EE-B952-1117DB460724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7718630E-FB7C-45B1-8640-5E76BDC97066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -176,9 +176,6 @@
     <t>Explained in Notes ?</t>
   </si>
   <si>
-    <t xml:space="preserve">yes </t>
-  </si>
-  <si>
     <t>733. Flood Fill</t>
   </si>
   <si>
@@ -239,12 +236,6 @@
     <t>https://leetcode.com/problems/surrounded-regions</t>
   </si>
   <si>
-    <t>Level by level , Required nearest . A - find nearest 1 from a zero value cell . Add 1 numbered cell with distance as zero initially and traverse its adj. where value is 0 and update distance every time</t>
-  </si>
-  <si>
-    <t>A - Traverse all 0 cells present on the edges and start DFS from each and mark their adjacent 0 cell's as can't convertible (#). Rest all will be  surronded X after dfs calls mark them as X</t>
-  </si>
-  <si>
     <t>DFS</t>
   </si>
   <si>
@@ -254,9 +245,6 @@
     <t>https://leetcode.com/problems/word-ladder</t>
   </si>
   <si>
-    <t xml:space="preserve">Hint- each word has difference of only one letter . We can comsider it as level . Approch - initially add beginword in queue as level1  and traverse every letter of a beginword and try replacing it by a-z and check if we can found our word for next level . </t>
-  </si>
-  <si>
     <t>Medium-Hard</t>
   </si>
   <si>
@@ -279,6 +267,90 @@
   </si>
   <si>
     <t>BFS , Graph - 126.Word Ladder II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS , Multiforce </t>
+  </si>
+  <si>
+    <t>BFS , Multiforce BFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of islands II </t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/number-of-islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes - page no.6 </t>
+  </si>
+  <si>
+    <t>TC and SC</t>
+  </si>
+  <si>
+    <t>TC - O(n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC - O(n) , SC - O(n) where n - number of nodes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC - O(n) , SC - O(n)- if all elemenets are at second level &amp; present in the queue. where n - number of nodes </t>
+  </si>
+  <si>
+    <t>yes - page no.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use recurrsion </t>
+  </si>
+  <si>
+    <t>yes - page no.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC - O(n*n*4) , SC - O(n*n)  - if all oranges are rotten </t>
+  </si>
+  <si>
+    <t>TC - O(n*n*4)- if all element contains org. color .               SC - O(N*M) -  to copy org. array , queue space</t>
+  </si>
+  <si>
+    <t>TC - O(n*n*4) - in case where all cells are 0 zero .      SC-0(n*n)</t>
+  </si>
+  <si>
+    <t>Level by level , Required nearest .                                                 A - find nearest 1 from a zero value cell . Add 1 numbered cell with distance as zero initially and traverse its adj. where value is 0 and update distance every time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A - Traverse all 0 cells present on the edges and start DFS from each and mark their adjacent 0 cell's as can't convertible (#).                      After DFS calls Rest all cell with 0 will be  surronded X . </t>
+  </si>
+  <si>
+    <t>TC - O(n*m) - each cell is visited at most once during DFS.                                                 SC - O(n*m) - recurrsion stack space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hint - each word has difference of only one letter .                  We can consider it as level .                      Approch - initially add beginword in queue as level1  and traverse every letter of a beginword and try replacing it by a-z and check if we can found our word for next level . </t>
+  </si>
+  <si>
+    <t>yes - page no.20</t>
+  </si>
+  <si>
+    <t>yes - page no.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC - O(N*L*26) - to tranverse the sequence and store it into the map .                             O(P*L*26) - P = no. shortest sequences and L - length of each word </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TC - O(N*L*26) - N length of list and L is of word .                           SC - O(N)</t>
+  </si>
+  <si>
+    <t>if we start bfs/dfs from any position of a island and visit its all land . We can traverse all islands like this and do count++ each time when we traversal is done for an islands</t>
+  </si>
+  <si>
+    <t>TC - O(n*m) - we are visiting each cell atmost once .            SC  - O(1)</t>
+  </si>
+  <si>
+    <t>yes - page no.33</t>
+  </si>
+  <si>
+    <t>yes -  page no.15</t>
+  </si>
+  <si>
+    <t>yes - page no.27</t>
   </si>
 </sst>
 </file>
@@ -662,10 +734,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -749,10 +821,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -840,10 +912,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -931,10 +1003,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -974,13 +1046,13 @@
     </row>
     <row r="3" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -989,13 +1061,13 @@
         <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1009,27 +1081,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" customWidth="1"/>
-    <col min="6" max="8" width="17.54296875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.6328125" customWidth="1"/>
+    <col min="3" max="4" width="26.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="9" width="17.54296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1040,34 +1112,37 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -1075,224 +1150,302 @@
         <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="8" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="116" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="L8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="I9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="L11" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://takeuforward.org/plus/dsa/problems/connected-components" xr:uid="{CBDDA4D9-3DA6-42F4-BD81-6766CE6059E4}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D4ED72D4-0FD6-484E-AD61-CDBC7D2FE01F}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{204D35F7-0D7E-417F-A9DE-9F302C399A4B}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{D9D07E69-64E9-4025-BC2E-109F77A1A0EB}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{CB99155B-7F58-442B-B942-44C03B0D3948}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{6B88E864-EB7E-4674-83FB-C291EEEF86E8}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{707A2146-0C97-4AFF-A5DE-34EB9AA17707}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{D4ED72D4-0FD6-484E-AD61-CDBC7D2FE01F}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{204D35F7-0D7E-417F-A9DE-9F302C399A4B}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{D9D07E69-64E9-4025-BC2E-109F77A1A0EB}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{CB99155B-7F58-442B-B942-44C03B0D3948}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{6B88E864-EB7E-4674-83FB-C291EEEF86E8}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{707A2146-0C97-4AFF-A5DE-34EB9AA17707}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{8471784A-FDFA-48E4-8240-4A6D4A9C9E1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated sheet for G-27 Shortest path in DAG
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF49DE-CB05-47EB-90AC-8E290B8BB1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6B4139-9E25-4302-9D64-D6B96C4A1060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
     <sheet name="Graph" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Graph!$A$1:$N$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="160">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -140,9 +143,6 @@
   </si>
   <si>
     <t>https://takeuforward.org/plus/dsa/problems/traversal-techniques</t>
-  </si>
-  <si>
-    <t>Use adjacency list , visited array and  traverse queue</t>
   </si>
   <si>
     <t>https://takeuforward.org/plus/dsa/problems/connected-components , https://leetcode.com/problems/number-of-provinces</t>
@@ -164,15 +164,9 @@
     <t>994. Rotting Oranges</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/rotting-oranges</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Hints - "adjacents\neighbors"  becomes rotten every min. Approch /Notes - https://leetcode.com/problems/rotting-oranges/solutions/7484164/easiest-explanation-in-simple-language-w-se3d/</t>
-  </si>
-  <si>
     <t>Explained in Notes ?</t>
   </si>
   <si>
@@ -182,12 +176,6 @@
     <t>https://leetcode.com/problems/flood-fill</t>
   </si>
   <si>
-    <t xml:space="preserve">for each unvisited node traverse all its neighbors using recurrsion and mark it as visited and return for how many unvisited nodes  you travelled </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use BFS/DFS </t>
-  </si>
-  <si>
     <t>BFS , DFS</t>
   </si>
   <si>
@@ -269,9 +257,6 @@
     <t>BFS , Graph - 126.Word Ladder II</t>
   </si>
   <si>
-    <t xml:space="preserve">BFS , Multiforce </t>
-  </si>
-  <si>
     <t>BFS , Multiforce BFS</t>
   </si>
   <si>
@@ -287,30 +272,15 @@
     <t>TC and SC</t>
   </si>
   <si>
-    <t xml:space="preserve">TC - O(n) , SC - O(n) where n - number of nodes </t>
-  </si>
-  <si>
     <t>yes - page no.8</t>
   </si>
   <si>
-    <t xml:space="preserve">use recurrsion </t>
-  </si>
-  <si>
     <t>yes - page no.11</t>
   </si>
   <si>
     <t xml:space="preserve">TC - O(n*n*4) , SC - O(n*n)  - if all oranges are rotten </t>
   </si>
   <si>
-    <t>TC - O(n*n*4)- if all element contains org. color .               SC - O(N*M) -  to copy org. array , queue space</t>
-  </si>
-  <si>
-    <t>TC - O(n*n*4) - in case where all cells are 0 zero .      SC-0(n*n)</t>
-  </si>
-  <si>
-    <t>Level by level , Required nearest .                                                 A - find nearest 1 from a zero value cell . Add 1 numbered cell with distance as zero initially and traverse its adj. where value is 0 and update distance every time</t>
-  </si>
-  <si>
     <t xml:space="preserve">A - Traverse all 0 cells present on the edges and start DFS from each and mark their adjacent 0 cell's as can't convertible (#).                      After DFS calls Rest all cell with 0 will be  surronded X . </t>
   </si>
   <si>
@@ -351,12 +321,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bipartite ? If graph doesn't contain cycle or if contain its length or no. edges present in a cycle are even . A - start coloring the graph and if you found any node </t>
-  </si>
-  <si>
-    <t>TC - O(v+e) - scan the edges to discover neighbors.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC - O(v+e) , SC - O(n)- if all elemenets are at second level &amp; present in the queue. where n - number of nodes </t>
   </si>
   <si>
     <t>TC - O(V+E)</t>
@@ -489,12 +453,503 @@
   <si>
     <t>yes - page no.54</t>
   </si>
+  <si>
+    <t>https://github.com/satyam-learning-log/DSA/blob/master/DSA_TOPICS/Graph/DFS.java</t>
+  </si>
+  <si>
+    <t>Easy-Medium</t>
+  </si>
+  <si>
+    <t>Recurrsion</t>
+  </si>
+  <si>
+    <t>Confidence (1-5)</t>
+  </si>
+  <si>
+    <t>TC - O(V+E) - scan the edges to discover neighbors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC - O(V+E) , SC - O(N)- queue </t>
+  </si>
+  <si>
+    <t>#1-25-01-25</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUITION:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Go as deep as possible from a node before backtracking to explore other paths .                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  - Mark node as visited .                                             - Recursively call DFS on its adjacent nodes, going as deep as possible before visiting other adjacents.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUITION:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Each DFS call covers exactly one connected component, so the number of times I start DFS from an unvisited node equals the number of components.                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH:   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                       
+- Iterate over all nodes.                                               - If a node is unvisited, start DFS from it to mark all nodes in that connected component.
+- Increment the count each time DFS is started from an unvisited node.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUITION:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For every rotten organes , after each min "adjancent" oraganes gets rotten.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                              APPROCH:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Count all fresh and rotten organes .                                           - Check  if it's possible to rotte fresh oranges .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-  Add all rotten oragnes (i,j) intially in the queue .                                              -For each rotten orange add it's 4-directionally adjacent to the queue as rotten orange for next min. and reduce count of fresh orange                                               - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Repeat this while queue is not empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- return min is fresh organes count == 0 else -1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MISTAKES:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DFS fails because it goes deep and delays other sources of rotten oranges . Single source bfs fail because multiple sources of rotten oranges spread at the same time .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                            </t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotting-oranges/solutions/7484164/easiest-explanation-in-simple-language-w-se3d/</t>
+  </si>
+  <si>
+    <t>TC - O(n*m*4)- worst case if all element contains org. color.            SC - O(N*M) -  to copy org. array , queue space.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUITION:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Explore the graph level by level by visiting all immediate neighbors first before going deep .                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH:   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Initially add starting node in a queue and mark it as visited.                                              -While queue is not empty  pop element from queue                      - Visit all it's adjacent neighbors and insert unvisited node into queue .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUTIONS :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Starting from source cell , spread new colour to its all adjacent and connected cell , Which has original colour until connected cells has original color .                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APPROCH:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Use Can DFS/BFS as expection is updated matrix.          - Start DFS/BFS from source cell .  - Visit it's adjacent cells and update it to new color.                                                    - Repeat this process until no orginal color cells found.</t>
+    </r>
+  </si>
+  <si>
+    <t>TC - O(n*n*4) - In worst case all cells are zero.               SC-0(n*n) - visited and distance matrix</t>
+  </si>
+  <si>
+    <t>#1-26-01-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ATOZ_G-27_Shortest_Path_In_Directed_Acyclic_Graph</t>
+  </si>
+  <si>
+    <r>
+      <t>INTUTION :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> In DAG , topological sort ensures the order to visit and calcuting min.cost by visiting it sequencally solve this .               </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH:                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Build the adjacency list with edge weights and compute the indegree array.                                                 - Perform topological sort to get nodes in valid processing order.                                                      - Initialize a distance (min cost) array with INF and set source distance to 0.                                                        - Start traversing queue from source retrived by topological sort .                                                  - For each node, relax all outgoing edges: (Poll node , traverse it's adjacents and update their cost)
+  dist[neighbor] = min(dist[neighbor], dist[current] + weight(current → neighbor)).                                          - Repeat this while queue is not empty.              </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC - O(V+E)                                 SC - O(V+E) - Queue , Indgree , Adjacency list </t>
+  </si>
+  <si>
+    <t>TC - O(V+E)    - Edges are distributed across vertices, not repeated for each vertex.                                            -0 → [1, 2]
+1 → [3]
+2 → []
+3 → [4]
+4 → []                                                     -Vertex - 4 , Edges - 2 + 1 + 0 + 1 + 0 = 4 = 4+4                                           SC - O(V) - Visited Array</t>
+  </si>
+  <si>
+    <t>BFS , Topological sort , Shortest Path</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +968,27 @@
     <font>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -539,7 +1015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -551,8 +1027,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -874,10 +1364,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -961,10 +1451,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -1052,10 +1542,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -1143,10 +1633,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -1186,13 +1676,13 @@
     </row>
     <row r="3" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1201,13 +1691,13 @@
         <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1221,641 +1711,733 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.08984375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="26.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
-    <col min="7" max="9" width="17.54296875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.54296875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.6328125" customWidth="1"/>
+    <col min="1" max="1" width="25.90625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="43.26953125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.7265625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" style="9" customWidth="1"/>
+    <col min="7" max="10" width="17.54296875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.453125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17.54296875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="17.6328125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="5">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="174" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="391.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="5">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="K13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="J14" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="116" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="16" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="116" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="145" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="G16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="203" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="116" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="M18" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="J19" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>122</v>
+      <c r="K19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="377" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="5">
+        <v>3</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N19" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://takeuforward.org/plus/dsa/problems/connected-components" xr:uid="{CBDDA4D9-3DA6-42F4-BD81-6766CE6059E4}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{D4ED72D4-0FD6-484E-AD61-CDBC7D2FE01F}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{204D35F7-0D7E-417F-A9DE-9F302C399A4B}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{D9D07E69-64E9-4025-BC2E-109F77A1A0EB}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{CB99155B-7F58-442B-B942-44C03B0D3948}"/>
-    <hyperlink ref="B8" r:id="rId6" xr:uid="{6B88E864-EB7E-4674-83FB-C291EEEF86E8}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{707A2146-0C97-4AFF-A5DE-34EB9AA17707}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{8471784A-FDFA-48E4-8240-4A6D4A9C9E1D}"/>
-    <hyperlink ref="B14" r:id="rId9" xr:uid="{A0ADA497-34FE-40D8-BD79-CFC4DD7CD22D}"/>
-    <hyperlink ref="B15" r:id="rId10" xr:uid="{64E0CAC4-AF4C-4BC0-A5F4-ED32F3C1AE7B}"/>
-    <hyperlink ref="B17" r:id="rId11" xr:uid="{7F63AB1E-05B1-467A-956D-9E3B4DE32E25}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{D9D07E69-64E9-4025-BC2E-109F77A1A0EB}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{CB99155B-7F58-442B-B942-44C03B0D3948}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{6B88E864-EB7E-4674-83FB-C291EEEF86E8}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{707A2146-0C97-4AFF-A5DE-34EB9AA17707}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{8471784A-FDFA-48E4-8240-4A6D4A9C9E1D}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{A0ADA497-34FE-40D8-BD79-CFC4DD7CD22D}"/>
+    <hyperlink ref="B15" r:id="rId9" xr:uid="{64E0CAC4-AF4C-4BC0-A5F4-ED32F3C1AE7B}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{7F63AB1E-05B1-467A-956D-9E3B4DE32E25}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{64E8EFF8-A9B6-4999-A422-5F2702B3E477}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{204D35F7-0D7E-417F-A9DE-9F302C399A4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solved shortest path in undirected graph
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618EAD74-2606-4A93-9615-6387738C6507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CDF562-9B17-4745-9F9C-0278F23A2DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Recurrsion" sheetId="3" r:id="rId3"/>
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
     <sheet name="Graph" sheetId="5" r:id="rId5"/>
+    <sheet name="LinkedList" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Graph!$A$1:$N$19</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="165">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -994,6 +995,9 @@
   </si>
   <si>
     <t>TC - O(V+E) SC - O(N)</t>
+  </si>
+  <si>
+    <t>82. Remove Duplicates from Sorted List II</t>
   </si>
 </sst>
 </file>
@@ -1764,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1773,7 +1777,7 @@
     <col min="1" max="1" width="25.90625" style="5" customWidth="1"/>
     <col min="2" max="2" width="43.26953125" style="5" customWidth="1"/>
     <col min="3" max="3" width="27.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.26953125" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" style="9" customWidth="1"/>
     <col min="5" max="5" width="17.7265625" style="9" customWidth="1"/>
     <col min="6" max="6" width="17.6328125" style="9" customWidth="1"/>
     <col min="7" max="10" width="17.54296875" style="5" customWidth="1"/>
@@ -1794,7 +1798,7 @@
       <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>78</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -1838,7 +1842,7 @@
       <c r="C2" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>158</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -1876,7 +1880,7 @@
       <c r="C3" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>142</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1911,7 +1915,7 @@
       <c r="C4" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>143</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -1981,7 +1985,7 @@
       <c r="C6" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>149</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -2016,7 +2020,7 @@
       <c r="C7" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -2054,7 +2058,7 @@
       <c r="C8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>83</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2086,7 +2090,7 @@
       <c r="C9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -2118,7 +2122,7 @@
       <c r="C10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2150,7 +2154,7 @@
       <c r="C11" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -2182,7 +2186,7 @@
       <c r="C12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>96</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -2214,7 +2218,7 @@
       <c r="C13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -2249,7 +2253,7 @@
       <c r="C14" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>101</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2281,7 +2285,7 @@
       <c r="C15" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>105</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -2313,7 +2317,7 @@
       <c r="C16" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -2345,7 +2349,7 @@
       <c r="C17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="5" t="s">
         <v>123</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -2377,7 +2381,7 @@
       <c r="C18" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2412,7 +2416,7 @@
       <c r="C19" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2485,7 +2489,7 @@
       <c r="C21" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="5" t="s">
         <v>163</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -2528,4 +2532,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D90093C-235B-4BFA-AC06-070A87C8F0C6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Solved L1631 Path with minimum efforts
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581A52AA-9548-44CB-86DE-CAFFF9C53291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6F6A02-98A3-4E7B-8ADF-632AD8D24A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="189">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -1330,6 +1330,71 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1631 . Path with minimum effort </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-with-minimum-effort/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUTION :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Try to traverse the graph by always selecting the node with minimum effort .For each node, store the maximum effort required to reach it from the source . 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APPROCH :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+- Initialize a priority queue with the source cell (effort = 0, row = 0, col = 0).
+- Maintain a matrix to store the minimum effort required to reach each cell. 
+- While the p queue != empty: 
+- - Extract the cell ,if it's  destination, return its effort . 
+- -  For each adjacent cell, compute the effort to reach it as:
+    max(current_effort, abs(height_diff)).
+- -  If this effort is smaller than the previously stored effort, update it and push the cell into the queue.
+- Continue until the destination is reached.</t>
+    </r>
+  </si>
+  <si>
+    <t>TC - O(4*m*N*log(N*M))
+- As exploring 4 path for each cell and pushing in pq . 
+SC - O(N*M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dijkstra's Algo. , BFS </t>
   </si>
 </sst>
 </file>
@@ -2105,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2905,7 +2970,7 @@
         <v>43</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="H23" s="5">
         <v>3</v>
@@ -2943,6 +3008,38 @@
         <v>3</v>
       </c>
       <c r="K24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="406" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H25" s="5">
+        <v>3</v>
+      </c>
+      <c r="K25" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2965,9 +3062,10 @@
     <hyperlink ref="B21" r:id="rId14" xr:uid="{CEDAAA7E-5F1D-468E-9B81-03C140F99175}"/>
     <hyperlink ref="B23" r:id="rId15" xr:uid="{31C8B4A9-695D-4CF3-863A-8252F2E49CF0}"/>
     <hyperlink ref="B24" r:id="rId16" xr:uid="{6F934A90-86CA-4917-897E-3423D55AA7C3}"/>
+    <hyperlink ref="B25" r:id="rId17" xr:uid="{D2C2ADDA-F55C-4908-966F-09CAB6F28365}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solved graph and sliding window problem
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0B75D3-B768-41A3-A6DA-192BCF4C88A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62BA0F4-A201-431F-B601-ADAFFAA0432B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
     <sheet name="Graph" sheetId="5" r:id="rId5"/>
     <sheet name="LinkedList" sheetId="6" r:id="rId6"/>
+    <sheet name="Sliding Window" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Graph!$A$1:$N$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Graph!$A$1:$N$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Sliding Window'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="212">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -473,9 +475,6 @@
     <t xml:space="preserve">TC - O(V+E) , SC - O(N)- queue </t>
   </si>
   <si>
-    <t>#1-25-01-25</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -886,12 +885,6 @@
   </si>
   <si>
     <t>TC - O(n*n*4) - In worst case all cells are zero.               SC-0(n*n) - visited and distance matrix</t>
-  </si>
-  <si>
-    <t>#1-26-01-25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>ATOZ_G-27_Shortest_Path_In_Directed_Acyclic_Graph</t>
@@ -1539,6 +1532,279 @@
   </si>
   <si>
     <t>Dijkstra's algo , BFS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INTUTION : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Starting from all zero cells, expanding level by level updates the minimum distance to the nearest zero.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH : 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Since there can be multiple zero cells (multiple sources), use multi-source BFS.
+- Initialize a queue , visited array and a distance matrix to store the distance of each cell from the nearest zero.
+- Add all zero cells to the queue with distance 0.
+- While the queue is not empty:
+  - Pop a cell from the queue.
+  - Explore its adjacent cells.
+  - If an adjacent cell has value 1 and "its distance is not yet set".
+    - Update its distance as current distance + 1.
+    - Add it to the queue for further exploration.
+- Continue until the queue is empty.
+- Return the distance matrix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTES :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No need to use visited array to prevent mutiple updates for already visited cell . we can use distance from that as well .</t>
+    </r>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>Revision (#1-26-01-25)</t>
+  </si>
+  <si>
+    <t>#1-04-02-26</t>
+  </si>
+  <si>
+    <t>#1-26-01-26</t>
+  </si>
+  <si>
+    <t>#1-25-01-26</t>
+  </si>
+  <si>
+    <t>1976. Number of Ways to Arrive at Destination</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-ways-to-arrive-at-destination</t>
+  </si>
+  <si>
+    <t>TC - O (E log V)
+SC - O (E+V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium - hard </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUTION :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Count for each node how many times we reached with min. distance . 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH : 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Initialze a pq with source , dis =0 , cost with Long.MAX and a mindisways array with source = 1  where we will store ways to reach node with min.distance   . 
+- Iterate over queue while it's not empty . 
+- - explore neighbors for current node . 
+- - if (dis[neighbor]&gt;currfornode+currtonode) then update mindisways[neighbor] =mindisways[current] and add neighbor in the queue
+-- else if (dis[neighbor]==currfornode+currtonode) then mindisways[neighbor] +=mindisways[current]
+- return mindisways[destination].
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTES: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>we need to store ways to reach the node with min. distance . (see note book ).</t>
+    </r>
+  </si>
+  <si>
+    <t>3634.Minimum Removals to Balance Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-removals-to-balance-array/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">INTUTION : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">If we can find a group (window) of elements that already satisfies the balance condition,Then all other elements can be removed.
+So the problem reduces to:
+Find the largest valid window → minimum removals
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH : 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Sort the array.
+- Traverse from left index i.
+- For each i, find the farthest index j such that : 
+nums[j] ≤ nums[i] * k.
+- Use binary search to find j
+- Calculate window size:
+window = j - i + 1
+- Removals needed:
+removals = n - window.
+- Track and return minimum removals across all windows</t>
+    </r>
+  </si>
+  <si>
+    <t>TC - O(N log N)</t>
+  </si>
+  <si>
+    <t>Sliding Window , Binary Search</t>
   </si>
 </sst>
 </file>
@@ -2314,11 +2580,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2363,7 +2629,7 @@
         <v>141</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>44</v>
@@ -2389,10 +2655,10 @@
         <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>38</v>
@@ -2407,7 +2673,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>77</v>
@@ -2427,7 +2693,7 @@
         <v>138</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>142</v>
@@ -2445,7 +2711,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>80</v>
@@ -2462,7 +2728,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>143</v>
@@ -2480,7 +2746,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>79</v>
@@ -2494,10 +2760,10 @@
         <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>81</v>
@@ -2515,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>49</v>
@@ -2532,10 +2798,10 @@
         <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>48</v>
@@ -2550,7 +2816,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>49</v>
@@ -2559,7 +2825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>58</v>
       </c>
@@ -2567,10 +2833,10 @@
         <v>59</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>24</v>
@@ -2585,7 +2851,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>85</v>
@@ -2992,16 +3258,16 @@
     </row>
     <row r="20" spans="1:13" ht="377" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>32</v>
@@ -3010,13 +3276,13 @@
         <v>43</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H20" s="5">
         <v>3</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>32</v>
@@ -3030,16 +3296,16 @@
     </row>
     <row r="21" spans="1:13" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>32</v>
@@ -3062,16 +3328,16 @@
     </row>
     <row r="22" spans="1:13" ht="261" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>32</v>
@@ -3080,7 +3346,7 @@
         <v>43</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H22" s="5">
         <v>4</v>
@@ -3089,24 +3355,24 @@
         <v>32</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>32</v>
@@ -3115,7 +3381,7 @@
         <v>43</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H23" s="5">
         <v>3</v>
@@ -3129,16 +3395,16 @@
     </row>
     <row r="24" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>32</v>
@@ -3147,7 +3413,7 @@
         <v>43</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H24" s="5">
         <v>3</v>
@@ -3156,21 +3422,21 @@
         <v>32</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="406" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>32</v>
@@ -3179,7 +3445,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H25" s="5">
         <v>3</v>
@@ -3190,16 +3456,16 @@
     </row>
     <row r="26" spans="1:13" ht="319" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>32</v>
@@ -3208,7 +3474,7 @@
         <v>43</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H26" s="5">
         <v>3</v>
@@ -3222,41 +3488,79 @@
     </row>
     <row r="27" spans="1:13" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="E27" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H27" s="5">
         <v>4</v>
       </c>
+      <c r="I27" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="K27" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H28" s="5">
+        <v>3</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N19" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}"/>
+  <autoFilter ref="A1:N27" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://takeuforward.org/plus/dsa/problems/connected-components" xr:uid="{CBDDA4D9-3DA6-42F4-BD81-6766CE6059E4}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{D4ED72D4-0FD6-484E-AD61-CDBC7D2FE01F}"/>
@@ -3276,9 +3580,10 @@
     <hyperlink ref="B24" r:id="rId16" xr:uid="{6F934A90-86CA-4917-897E-3423D55AA7C3}"/>
     <hyperlink ref="B25" r:id="rId17" xr:uid="{D2C2ADDA-F55C-4908-966F-09CAB6F28365}"/>
     <hyperlink ref="B26" r:id="rId18" xr:uid="{8A5A832F-666A-493E-A3EB-1DD4476A0B7B}"/>
+    <hyperlink ref="B28" r:id="rId19" xr:uid="{5CEB0A28-62E3-4F7D-9DA7-371B1C990640}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -3355,16 +3660,16 @@
     </row>
     <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>24</v>
@@ -3373,19 +3678,19 @@
         <v>43</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H2" s="9">
         <v>3</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3396,4 +3701,109 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBB5AD9-6759-49B8-8C85-DCC62C1F65FC}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O1" xr:uid="{2BBB5AD9-6759-49B8-8C85-DCC62C1F65FC}"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{78E200A1-F1DC-4FA8-ACD2-EB3A411CCC64}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
solved - MultiSourceShortestPath - floyd warsholl
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2026\learninglog\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD53691-A21A-4527-ADED-75541F2DF64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82414212-B978-4B9C-9A31-A2A6C49AE4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,13 @@
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
     <sheet name="Graph" sheetId="5" r:id="rId5"/>
     <sheet name="LinkedList" sheetId="6" r:id="rId6"/>
-    <sheet name="Sliding Window" sheetId="7" r:id="rId7"/>
+    <sheet name="Subarray" sheetId="8" r:id="rId7"/>
+    <sheet name="Sliding Window" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Graph!$A$1:$N$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Sliding Window'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Sliding Window'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Subarray!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="235">
   <si>
     <t xml:space="preserve">Problem Name </t>
   </si>
@@ -282,9 +284,6 @@
   </si>
   <si>
     <t xml:space="preserve">TC - O(n*n*4) , SC - O(n*n)  - if all oranges are rotten </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A - Traverse all 0 cells present on the edges and start DFS from each and mark their adjacent 0 cell's as can't convertible (#).                      After DFS calls Rest all cell with 0 will be  surronded X . </t>
   </si>
   <si>
     <t>TC - O(n*m) - each cell is visited at most once during DFS.                                                 SC - O(n*m) - recurrsion stack space</t>
@@ -1813,15 +1812,176 @@
     <t>https://takeuforward.org/dsa/strivers-a2z-sheet-learn-dsa-a-to-z</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">NEED : Dijkstra don't work on negative edges and give tle in case of negative cycle in the graph . 
+    <t>TC - O(N*E)
+SC - O(N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>3835. Count Subarrays With Cost Less Than or Equal to K</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-subarrays-with-cost-less-than-or-equal-to-k</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INTUITION:
+By maintaining a valid sliding window and tracking its minimum and maximum, we can count all subarrays as we add each new index.
+APPROACH:
+- We need to track the minimum value, maximum value, and window length to maintain a valid window.
+- Using only min/max heaps (even with indices) is not sufficient because we must efficiently shrink the window based on index order.
+- Use two monotonic deques:
+  - A decreasing deque to track the maximum values.
+  - An increasing deque to track the minimum values.
+- Expand the window by adding the right index:
+  - Update both deques by removing invalid elements from the back.
+- While the window becomes invalid (cost &gt; k):
+  - Shrink the window from the left.
+  - Remove indices from the front of deques if they go out of the window.
+- For each valid window ending at right, add (right − left + 1) to the answer.
+- Continue until all indices are processed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTES : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Please see the notes 
+</t>
+    </r>
+  </si>
+  <si>
+    <t>O(N) - Each element is added once to the min deque and max deque.
+Each element is removed at most once from each deque.
+Left and right pointers both move forward only.</t>
+  </si>
+  <si>
+    <t>Subarray , Sliding window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - Subarray </t>
+  </si>
+  <si>
+    <t>2 - Sliding window</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUITION:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+By maintaining a valid sliding window and tracking its minimum and maximum, we can count all subarrays as we add each new index.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APPROACH:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Use two monotonic deques:
+  - A decreasing deque to track the maximum values.
+  - An increasing deque to track the minimum values.
+- Expand the window by adding the right index:
+  - Update both deques by removing invalid elements from the back.
+- While the window becomes invalid (cost &gt; k):
+  - Shrink the window from the left.
+  - Remove indices from the front of deques if they go out of the window.
+- For each valid window ending at right, add (right − left + 1) to the answer.
+- Continue until all indices are processed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTES : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please see the notes . 
+- We need to track the minimum value, maximum value, and window length to maintain a valid window.
+- Using only min/max heaps (even with indices) is not sufficient because we must efficiently shrink the window based on index order.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUTION :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Any 0 connected to the boundary and 0 cell's adjacent to it cannot be surrounded , and remaining 0 are surrounded by X . 
 </t>
     </r>
     <r>
@@ -1843,7 +2003,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- Intialize the cost with MAX except Source node .</t>
+      <t>- Start dfs from every 0 cell on boundry . 
+- visit their adjacents 0's and mark as not capturable . 
+- After performing  all dfs ,  remaining 0 cell's will be surronded by X . 
+- convert remaining cells to X 
+- return the matrix.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NEED : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dijkstra don't work on negative edges and gives tle in case of negative cycle in the graph . 
+</t>
     </r>
     <r>
       <rPr>
@@ -1853,7 +2040,74 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>APPROCH :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+- Intialize the cost with MAX except Source node .
+- Iterate over the edges totalnodes-1 times and update cost array for the node if we can reach it with minimum cost than previous.
+- while Iterating on edges Nth time if we find any updation then return saying "Cycle exists in the graph".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTES :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cycle in a graph which contain at least one negative edge doesn't means negative cycle . Sum of the cycle path must be less than zero to say "Negative Cycle".</t>
+    </r>
+  </si>
+  <si>
+    <t>https://takeuforward.org/data-structure/floyd-warshall-algorithm-g-42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floyd Warshall </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NOTES : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In this approch we check if there is any path to reach i -&gt; j via k i.e i-&gt;k-&gt;j to minimize its distance. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
+APPROCH : 
 </t>
     </r>
     <r>
@@ -1864,53 +2118,94 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- Iterate over the edges totalnodes-1 times and update cost array for the node if we can reach it with minimum cost than previous.
-- while Iterating on edges Nth time if we find any updation then return saying "Cycle exists in the graph".</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Initialize a distance matrix to store the minimum distance between each pair of nodes, using the adjacency matrix of the graph. If there is an edge between two nodes, set the corresponding distance; if no edge exists, set the distance to infinity (or a large value).
+- Iterate through all possible nodes as intermediate nodes. For each intermediate node k, update the distance matrix by checking all pairs of nodes (i, j):
+- - If k is not an intermediate node in the path from i to j, skip that iteration.
+- - If there is no direct edge between i and j, update dist[i][j] to dist[i][k] + dist[k][j].
+- - If there is a direct edge between i and j, update dist[i][j] to the minimum of dist[i][j] and dist[i][k] + dist[k][j].
+- Continue iterating through all the possible intermediate nodes until the entire distance matrix is updated.
+- At the end of the process, the distance matrix will contain the shortest distances between all pairs of nodes. If a node is unreachable, its distance will remain as infinity (or -1 if used to denote unreachable nodes).</t>
+    </r>
+  </si>
+  <si>
+    <t>TC - O(n^3) - for each node we check i-&gt;k-&gt;j</t>
+  </si>
+  <si>
+    <t>1334. Find the City With the Smallest Number of Neighbors at a Threshold Distance</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-the-city-with-the-smallest-number-of-neighbors-at-a-threshold-distance/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTUTION :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> If we have with us  min. distance to reach each city from current , we can collect cities which match the threshold condition. 
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">NOTES : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cycle in a graph which contain at least one negative edge doesn't means negative cycle . Sum of the cycle path must be less than zero to say "Negative Cycle".</t>
-    </r>
-  </si>
-  <si>
-    <t>TC - O(N*E)
-SC - O(N)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Striver ATOZ </t>
-  </si>
-  <si>
-    <t>Shortest Path Algo.</t>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APPROCH : 
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate min. distance to reach each city from current using floyd warsholl . 
+- Initilize PQ to store city and no. cities which can be traversed with atmost threshold . 
+- Traverse the distance matrix and add city with no.cities which can be reached . 
+- return peek of pq .</t>
+    </r>
+  </si>
+  <si>
+    <t>TC - O(n^3)
+SC - O(n)</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +2265,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF002060"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1997,7 +2292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2025,6 +2320,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2693,11 +2991,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F4D11-A7C4-43BB-9B31-F105D2E4CA7B}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2739,10 +3037,10 @@
         <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>44</v>
@@ -2751,7 +3049,7 @@
         <v>13</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>10</v>
@@ -2768,10 +3066,10 @@
         <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>38</v>
@@ -2786,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>77</v>
@@ -2803,28 +3101,28 @@
         <v>63</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="H3" s="5">
         <v>5</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>80</v>
@@ -2841,10 +3139,10 @@
         <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>32</v>
@@ -2859,7 +3157,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>79</v>
@@ -2873,10 +3171,10 @@
         <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>81</v>
@@ -2894,7 +3192,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>49</v>
@@ -2911,10 +3209,10 @@
         <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>48</v>
@@ -2929,7 +3227,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>49</v>
@@ -2946,10 +3244,10 @@
         <v>59</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>24</v>
@@ -2964,10 +3262,10 @@
         <v>4</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>32</v>
@@ -2976,7 +3274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="232" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>61</v>
       </c>
@@ -2984,10 +3282,10 @@
         <v>62</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>24</v>
@@ -2999,7 +3297,7 @@
         <v>63</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>32</v>
@@ -3016,10 +3314,10 @@
         <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>25</v>
@@ -3031,7 +3329,7 @@
         <v>35</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>32</v>
@@ -3051,7 +3349,7 @@
         <v>68</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>25</v>
@@ -3063,7 +3361,7 @@
         <v>70</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>32</v>
@@ -3080,10 +3378,10 @@
         <v>76</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>32</v>
@@ -3095,7 +3393,7 @@
         <v>70</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>32</v>
@@ -3106,16 +3404,16 @@
     </row>
     <row r="12" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>32</v>
@@ -3127,7 +3425,7 @@
         <v>63</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>32</v>
@@ -3138,16 +3436,16 @@
     </row>
     <row r="13" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>32</v>
@@ -3159,30 +3457,30 @@
         <v>63</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>32</v>
@@ -3191,10 +3489,10 @@
         <v>43</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>32</v>
@@ -3205,16 +3503,16 @@
     </row>
     <row r="15" spans="1:14" ht="203" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>32</v>
@@ -3223,10 +3521,10 @@
         <v>43</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>32</v>
@@ -3237,16 +3535,16 @@
     </row>
     <row r="16" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>32</v>
@@ -3255,30 +3553,30 @@
         <v>43</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>32</v>
@@ -3287,30 +3585,30 @@
         <v>43</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="203" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>32</v>
@@ -3319,33 +3617,33 @@
         <v>43</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>32</v>
@@ -3354,33 +3652,33 @@
         <v>43</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="377" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>32</v>
@@ -3389,42 +3687,42 @@
         <v>43</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H20" s="5">
         <v>3</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>35</v>
@@ -3441,16 +3739,16 @@
     </row>
     <row r="22" spans="1:13" ht="261" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>32</v>
@@ -3459,7 +3757,7 @@
         <v>43</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H22" s="5">
         <v>4</v>
@@ -3468,24 +3766,24 @@
         <v>32</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>32</v>
@@ -3494,7 +3792,7 @@
         <v>43</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H23" s="5">
         <v>3</v>
@@ -3508,16 +3806,16 @@
     </row>
     <row r="24" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>32</v>
@@ -3526,7 +3824,7 @@
         <v>43</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H24" s="5">
         <v>3</v>
@@ -3535,21 +3833,21 @@
         <v>32</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="406" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>32</v>
@@ -3558,7 +3856,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H25" s="5">
         <v>3</v>
@@ -3569,16 +3867,16 @@
     </row>
     <row r="26" spans="1:13" ht="319" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>32</v>
@@ -3587,7 +3885,7 @@
         <v>43</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H26" s="5">
         <v>3</v>
@@ -3601,16 +3899,16 @@
     </row>
     <row r="27" spans="1:13" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>25</v>
@@ -3619,45 +3917,45 @@
         <v>43</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H27" s="5">
         <v>4</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H28" s="5">
         <v>3</v>
@@ -3666,10 +3964,94 @@
         <v>32</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H29" s="5">
+        <v>4</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="5">
+        <v>3</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="261" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H31" s="5">
+        <v>4</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3694,9 +4076,11 @@
     <hyperlink ref="B25" r:id="rId17" xr:uid="{D2C2ADDA-F55C-4908-966F-09CAB6F28365}"/>
     <hyperlink ref="B26" r:id="rId18" xr:uid="{8A5A832F-666A-493E-A3EB-1DD4476A0B7B}"/>
     <hyperlink ref="B28" r:id="rId19" xr:uid="{5CEB0A28-62E3-4F7D-9DA7-371B1C990640}"/>
+    <hyperlink ref="B29" r:id="rId20" xr:uid="{ED6D3629-9BAC-4F79-9135-D4EA70CC2E96}"/>
+    <hyperlink ref="B30" r:id="rId21" xr:uid="{6A758F7A-79FB-495C-B418-9EDF46598B5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -3749,7 +4133,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>50</v>
@@ -3761,7 +4145,7 @@
         <v>13</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>10</v>
@@ -3773,16 +4157,16 @@
     </row>
     <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>24</v>
@@ -3791,19 +4175,19 @@
         <v>43</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H2" s="9">
         <v>3</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3817,12 +4201,124 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97E19B9-CD82-4865-8D9B-AA4D0F508F84}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="21.26953125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="9"/>
+    <col min="11" max="11" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="9">
+        <v>3</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E5" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{C97E19B9-CD82-4865-8D9B-AA4D0F508F84}"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8D7A9693-6B31-4478-B435-F6054BBB9C05}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBB5AD9-6759-49B8-8C85-DCC62C1F65FC}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3838,11 +4334,11 @@
     <col min="9" max="9" width="17.81640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.6328125" style="2" customWidth="1"/>
     <col min="11" max="11" width="17.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" style="5" customWidth="1"/>
     <col min="13" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3865,10 +4361,10 @@
         <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>44</v>
@@ -3877,7 +4373,7 @@
         <v>13</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>10</v>
@@ -3888,16 +4384,16 @@
     </row>
     <row r="2" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>25</v>
@@ -3906,52 +4402,58 @@
         <v>43</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H2" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="L2" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="7"/>
+      <c r="L3" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" s="9">
+        <v>3</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H3" s="5">
-        <v>3</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>218</v>
+      <c r="L4" s="9" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{2BBB5AD9-6759-49B8-8C85-DCC62C1F65FC}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{78E200A1-F1DC-4FA8-ACD2-EB3A411CCC64}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{8A797BA2-6F35-4B96-90B3-EDDF17E0283E}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{A45A0E55-7AB9-485C-AA0D-19E5272C99AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>